<commit_message>
ADD: you can now generate multiple configs from an exel, yaml and j2 template
</commit_message>
<xml_diff>
--- a/TestFiles/TestDevices.xlsx
+++ b/TestFiles/TestDevices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmatt\Documents\Coding\Python\config-generator\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21A4FB1A-C804-415D-BCA8-86E5DB47E08E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BA69D9-6112-4C99-96BD-206D67100351}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{0458932A-CD27-40CA-A9D9-B02C2A0B97E4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t>STG</t>
+  </si>
+  <si>
+    <t>SW70</t>
+  </si>
+  <si>
+    <t>SW100</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>TUE</t>
   </si>
 </sst>
 </file>
@@ -391,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50DB75F5-C929-4A25-8471-1A039CECF976}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +433,28 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>556987</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>996874</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>